<commit_message>
Update Base ByteBank - Saldo do Cliente - Planilha Inicial.xlsx
</commit_message>
<xml_diff>
--- a/Excel/Avançado/VBA/Base ByteBank - Saldo do Cliente - Planilha Inicial.xlsx
+++ b/Excel/Avançado/VBA/Base ByteBank - Saldo do Cliente - Planilha Inicial.xlsx
@@ -1,42 +1,31 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
-  <workbookPr defaultThemeVersion="166925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
+  <workbookPr codeName="EstaPastaDeTrabalho" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://officeresolve-my.sharepoint.com/personal/r_sabino_officeresolve_com_br/Documents/Alura-Ciência de Dados/04 - Nova Formação VBA/3636 - VBA 1 - Automatizando tarefas do dia a dia/Materiais do Curso/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Desktop\exercicios\alura\Excel\Avançado\VBA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7820DD64-D4C5-4570-A4B8-A6E957E8BDA4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B2F6520-7A08-4BDB-A718-0DAD26E6A5CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{05CA96A6-47A0-4B3D-B939-EAC1B4F9044E}"/>
+    <workbookView xWindow="28692" yWindow="624" windowWidth="19416" windowHeight="11496" xr2:uid="{05CA96A6-47A0-4B3D-B939-EAC1B4F9044E}"/>
   </bookViews>
   <sheets>
     <sheet name="Dados_Importados" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="23">
   <si>
     <t>ID_Cliente</t>
   </si>
@@ -102,6 +91,9 @@
   </si>
   <si>
     <t>%Nome Cliente 1009</t>
+  </si>
+  <si>
+    <t>byte_1001</t>
   </si>
 </sst>
 </file>
@@ -476,18 +468,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{153E2180-7C80-483D-A8DD-7976CB8BFA50}">
+  <sheetPr codeName="Planilha1"/>
   <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="18.33203125" customWidth="1"/>
-    <col min="2" max="2" width="28.33203125" customWidth="1"/>
-    <col min="3" max="3" width="19.88671875" customWidth="1"/>
-    <col min="4" max="4" width="20.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.44140625" customWidth="1"/>
+    <col min="2" max="2" width="22.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
@@ -505,8 +498,8 @@
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2" s="2">
-        <v>1001</v>
+      <c r="A2" s="2" t="s">
+        <v>22</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>13</v>

</xml_diff>